<commit_message>
update tech radar data
</commit_message>
<xml_diff>
--- a/packages/app/public/techradar/data.xlsx
+++ b/packages/app/public/techradar/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tinnapat.c/github/tinnapat/devx-backstage/packages/app/public/techradar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{82491651-4B7A-E942-84C9-034239E1AEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EA66B0FF-58EA-E649-BE35-22934E841993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-43440" yWindow="2000" windowWidth="40960" windowHeight="16940"/>
+    <workbookView xWindow="-26920" yWindow="2000" windowWidth="24440" windowHeight="16940"/>
   </bookViews>
   <sheets>
     <sheet name="KBTG" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="191">
   <si>
     <t>name</t>
   </si>
@@ -85,15 +85,9 @@
     <t>Open API</t>
   </si>
   <si>
-    <t>Blue-green deployment</t>
-  </si>
-  <si>
     <t>AB/testing</t>
   </si>
   <si>
-    <t>Security exception</t>
-  </si>
-  <si>
     <t>SoAC</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
     <t>Code review</t>
   </si>
   <si>
-    <t>Trunk-based development</t>
-  </si>
-  <si>
     <t>TDD</t>
   </si>
   <si>
@@ -136,12 +127,6 @@
     <t>DBOps</t>
   </si>
   <si>
-    <t>Architecture-as-a-code</t>
-  </si>
-  <si>
-    <t>Canary deployment</t>
-  </si>
-  <si>
     <t>MongoDB</t>
   </si>
   <si>
@@ -157,9 +142,6 @@
     <t>Google Big Query</t>
   </si>
   <si>
-    <t>Openshift</t>
-  </si>
-  <si>
     <t>Docker</t>
   </si>
   <si>
@@ -175,72 +157,33 @@
     <t>Huawei Cloud</t>
   </si>
   <si>
-    <t>MS SQL</t>
-  </si>
-  <si>
     <t>MySql</t>
   </si>
   <si>
-    <t>Oracle</t>
-  </si>
-  <si>
     <t>Backstage.io</t>
   </si>
   <si>
-    <t>Main frame</t>
-  </si>
-  <si>
     <t>Hadoop</t>
   </si>
   <si>
     <t>IBM Cloud</t>
   </si>
   <si>
-    <t>Palo Alto FW</t>
-  </si>
-  <si>
-    <t>ELK</t>
-  </si>
-  <si>
     <t>Grafana</t>
   </si>
   <si>
-    <t>HPQC</t>
-  </si>
-  <si>
-    <t>UFT</t>
-  </si>
-  <si>
-    <t>Tufin (FW)</t>
-  </si>
-  <si>
     <t>Forcepoint DLP</t>
   </si>
   <si>
-    <t>One Drive</t>
-  </si>
-  <si>
-    <t>Prometheus Dynatrace</t>
-  </si>
-  <si>
     <t>Jenkins</t>
   </si>
   <si>
     <t>Azure AD</t>
   </si>
   <si>
-    <t>Load test performance center</t>
-  </si>
-  <si>
     <t>Robot Framework</t>
   </si>
   <si>
-    <t>Microsoft Outlook</t>
-  </si>
-  <si>
-    <t>Microsoft Office</t>
-  </si>
-  <si>
     <t>Libre Office</t>
   </si>
   <si>
@@ -307,9 +250,6 @@
     <t>EDR</t>
   </si>
   <si>
-    <t>C4 Diagram</t>
-  </si>
-  <si>
     <t>Slack</t>
   </si>
   <si>
@@ -415,21 +355,12 @@
     <t>AWS</t>
   </si>
   <si>
-    <t>Office 365</t>
-  </si>
-  <si>
-    <t>Windows</t>
-  </si>
-  <si>
     <t>Microsoft Teams</t>
   </si>
   <si>
     <t>Humatrix</t>
   </si>
   <si>
-    <t>Linux</t>
-  </si>
-  <si>
     <t>Android</t>
   </si>
   <si>
@@ -445,9 +376,6 @@
     <t>XCode</t>
   </si>
   <si>
-    <t>LoadRunner</t>
-  </si>
-  <si>
     <t>Prisma Cloud</t>
   </si>
   <si>
@@ -457,9 +385,6 @@
     <t>Quarterly Business Review</t>
   </si>
   <si>
-    <t>Hashicorp Vault</t>
-  </si>
-  <si>
     <t>JFrog</t>
   </si>
   <si>
@@ -478,30 +403,18 @@
     <t>Ansible</t>
   </si>
   <si>
-    <t>Postgres</t>
-  </si>
-  <si>
     <t>Nginx</t>
   </si>
   <si>
     <t>Security PDPA</t>
   </si>
   <si>
-    <t>VMWare</t>
-  </si>
-  <si>
-    <t>Elasticsearch</t>
-  </si>
-  <si>
     <t>GTM</t>
   </si>
   <si>
     <t>Team Topology</t>
   </si>
   <si>
-    <t>EA Framework</t>
-  </si>
-  <si>
     <t>Kafka</t>
   </si>
   <si>
@@ -517,9 +430,6 @@
     <t>Message Queue</t>
   </si>
   <si>
-    <t>Lucene</t>
-  </si>
-  <si>
     <t>J2EE</t>
   </si>
   <si>
@@ -556,16 +466,10 @@
     <t>WebSphere Application Server</t>
   </si>
   <si>
-    <t>Apigee</t>
-  </si>
-  <si>
     <t>MS Teams</t>
   </si>
   <si>
     <t>BurpSuite</t>
-  </si>
-  <si>
-    <t>Serive Virtualization</t>
   </si>
   <si>
     <t>BMC Control-M</t>
@@ -600,6 +504,96 @@
   </si>
   <si>
     <t>การใช้ LINE for Work แทนที่ LINE ในการคุยงาน จะทำให้ข้อมูลที่คุยกัน ทั้งรูปภาพ และ attachments ไม่หาย และมีความ secure ขึ้น ปัจจุบันยังอยู่ในการศึกษาเพิ่มเติมอยู่ concern ที่มีในขณะนี้มีแค่เรื่องค่าใช้จ่ายที่จะเกิดขึ้น ทีมใดสนใจ ติดต่อคุณกระทิง</t>
+  </si>
+  <si>
+    <t>Service Virtualization</t>
+  </si>
+  <si>
+    <t>OpenShift Container Platform</t>
+  </si>
+  <si>
+    <t>https://www.redhat.com/en/technologies/cloud-computing/openshift/container-platform</t>
+  </si>
+  <si>
+    <t>Dynatrace</t>
+  </si>
+  <si>
+    <t>Prometheus</t>
+  </si>
+  <si>
+    <t>Mainframe</t>
+  </si>
+  <si>
+    <t>Security Review</t>
+  </si>
+  <si>
+    <t>Blue-green Deployment</t>
+  </si>
+  <si>
+    <t>Apache Lucene</t>
+  </si>
+  <si>
+    <t>https://lucene.apache.org/</t>
+  </si>
+  <si>
+    <t>Architecture as Code</t>
+  </si>
+  <si>
+    <t>Trunk-based Development</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server</t>
+  </si>
+  <si>
+    <t>C4 Diagrams</t>
+  </si>
+  <si>
+    <t>HashiCorp Vault</t>
+  </si>
+  <si>
+    <t>https://www.delphix.com/</t>
+  </si>
+  <si>
+    <t>Micro Focus Quality Center</t>
+  </si>
+  <si>
+    <t>Micro Focus Performance Center</t>
+  </si>
+  <si>
+    <t>Micro Focus Unified Functional Testing</t>
+  </si>
+  <si>
+    <t>Apigee API Management</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/apigee</t>
+  </si>
+  <si>
+    <t>Canary Deployment</t>
+  </si>
+  <si>
+    <t>MS Office 365</t>
+  </si>
+  <si>
+    <t>Micro Focus LoadRunner</t>
+  </si>
+  <si>
+    <t>Elastic Stack</t>
+  </si>
+  <si>
+    <t>Oracle DB</t>
+  </si>
+  <si>
+    <t>Tufin Firewall Management</t>
+  </si>
+  <si>
+    <t>https://www.tufin.com/</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>VMWare ESXi</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1099,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1119,10 +1113,13 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1481,19 +1478,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F169"/>
+  <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="91.1640625" style="3" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -1509,12 +1506,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1531,9 +1528,9 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="3" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1550,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -1566,9 +1563,9 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="3" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1585,12 +1582,12 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1601,9 +1598,9 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="3" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -1620,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -1636,9 +1633,9 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="3" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -1655,12 +1652,12 @@
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -1671,9 +1668,9 @@
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="3" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1690,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1706,7 +1703,7 @@
       <c r="D12" s="2">
         <v>0</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -1724,7 +1721,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -1735,11 +1732,11 @@
       <c r="D14" s="2">
         <v>0</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
@@ -1753,7 +1750,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>167</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>5</v>
@@ -1764,11 +1761,11 @@
       <c r="D16" s="2">
         <v>0</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>5</v>
@@ -1782,7 +1779,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>5</v>
@@ -1793,11 +1790,11 @@
       <c r="D18" s="2">
         <v>0</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>5</v>
@@ -1811,7 +1808,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>172</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>5</v>
@@ -1822,11 +1819,11 @@
       <c r="D20" s="2">
         <v>0</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>5</v>
@@ -1840,7 +1837,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>5</v>
@@ -1851,11 +1848,11 @@
       <c r="D22" s="2">
         <v>0</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>5</v>
@@ -1869,7 +1866,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>5</v>
@@ -1883,7 +1880,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>5</v>
@@ -1894,11 +1891,11 @@
       <c r="D25" s="2">
         <v>0</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>5</v>
@@ -1912,7 +1909,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
@@ -1923,11 +1920,11 @@
       <c r="D27" s="2">
         <v>0</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>5</v>
@@ -1941,7 +1938,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>5</v>
@@ -1952,11 +1949,11 @@
       <c r="D29" s="2">
         <v>0</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>8</v>
@@ -1970,7 +1967,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>11</v>
@@ -1981,11 +1978,11 @@
       <c r="D31" s="2">
         <v>0</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>171</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>11</v>
@@ -1999,7 +1996,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>182</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>11</v>
@@ -2010,11 +2007,11 @@
       <c r="D33" s="2">
         <v>0</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>5</v>
@@ -2028,7 +2025,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>14</v>
@@ -2039,11 +2036,11 @@
       <c r="D35" s="2">
         <v>0</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>5</v>
@@ -2057,7 +2054,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>5</v>
@@ -2068,11 +2065,11 @@
       <c r="D37" s="2">
         <v>0</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>5</v>
@@ -2086,7 +2083,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>5</v>
@@ -2097,11 +2094,11 @@
       <c r="D39" s="2">
         <v>0</v>
       </c>
-      <c r="E39" s="2"/>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>5</v>
@@ -2113,9 +2110,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>5</v>
@@ -2126,11 +2123,13 @@
       <c r="D41" s="2">
         <v>0</v>
       </c>
-      <c r="E41" s="2"/>
+      <c r="E41" s="7" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>5</v>
@@ -2144,7 +2143,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>5</v>
@@ -2158,7 +2157,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>5</v>
@@ -2169,11 +2168,11 @@
       <c r="D44" s="2">
         <v>0</v>
       </c>
-      <c r="E44" s="2"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>5</v>
@@ -2187,7 +2186,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>5</v>
@@ -2198,11 +2197,11 @@
       <c r="D46" s="2">
         <v>0</v>
       </c>
-      <c r="E46" s="2"/>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>173</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>5</v>
@@ -2216,7 +2215,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>5</v>
@@ -2227,11 +2226,11 @@
       <c r="D48" s="2">
         <v>0</v>
       </c>
-      <c r="E48" s="2"/>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>186</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>5</v>
@@ -2245,7 +2244,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>11</v>
@@ -2256,11 +2255,11 @@
       <c r="D50" s="2">
         <v>0</v>
       </c>
-      <c r="E50" s="2"/>
+      <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>166</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>14</v>
@@ -2274,7 +2273,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>14</v>
@@ -2285,11 +2284,11 @@
       <c r="D52" s="2">
         <v>0</v>
       </c>
-      <c r="E52" s="2"/>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>14</v>
@@ -2303,7 +2302,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>5</v>
@@ -2314,11 +2313,11 @@
       <c r="D54" s="2">
         <v>0</v>
       </c>
-      <c r="E54" s="2"/>
+      <c r="E54" s="6"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>177</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
@@ -2332,7 +2331,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>179</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>5</v>
@@ -2343,11 +2342,11 @@
       <c r="D56" s="2">
         <v>0</v>
       </c>
-      <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>187</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>5</v>
@@ -2358,10 +2357,13 @@
       <c r="D57" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E57" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>180</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>5</v>
@@ -2372,11 +2374,13 @@
       <c r="D58" s="2">
         <v>0</v>
       </c>
-      <c r="E58" s="2"/>
+      <c r="E58" s="7" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>5</v>
@@ -2390,7 +2394,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>178</v>
+        <v>50</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>5</v>
@@ -2401,11 +2405,11 @@
       <c r="D60" s="2">
         <v>0</v>
       </c>
-      <c r="E60" s="2"/>
+      <c r="E60" s="6"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>5</v>
@@ -2413,28 +2417,29 @@
       <c r="C61" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D61" s="1">
-        <v>0</v>
-      </c>
+      <c r="D61" s="2">
+        <v>0</v>
+      </c>
+      <c r="E61" s="6"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="A62" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="2">
         <v>0</v>
       </c>
-      <c r="E62" s="2"/>
+      <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>5</v>
@@ -2448,7 +2453,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>5</v>
@@ -2459,11 +2464,11 @@
       <c r="D64" s="2">
         <v>0</v>
       </c>
-      <c r="E64" s="2"/>
+      <c r="E64" s="6"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>180</v>
+        <v>52</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>5</v>
@@ -2477,7 +2482,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>5</v>
@@ -2488,11 +2493,11 @@
       <c r="D66" s="2">
         <v>0</v>
       </c>
-      <c r="E66" s="2"/>
+      <c r="E66" s="6"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>68</v>
+        <v>178</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>5</v>
@@ -2506,7 +2511,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>181</v>
+        <v>53</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>5</v>
@@ -2517,11 +2522,11 @@
       <c r="D68" s="2">
         <v>0</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="6"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>5</v>
@@ -2535,7 +2540,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>5</v>
@@ -2546,11 +2551,11 @@
       <c r="D70" s="2">
         <v>0</v>
       </c>
-      <c r="E70" s="2"/>
+      <c r="E70" s="6"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>5</v>
@@ -2564,7 +2569,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>5</v>
@@ -2575,11 +2580,11 @@
       <c r="D72" s="2">
         <v>0</v>
       </c>
-      <c r="E72" s="2"/>
+      <c r="E72" s="6"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>5</v>
@@ -2593,7 +2598,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>5</v>
@@ -2604,11 +2609,11 @@
       <c r="D74" s="2">
         <v>0</v>
       </c>
-      <c r="E74" s="2"/>
+      <c r="E74" s="6"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>5</v>
@@ -2622,7 +2627,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>182</v>
+        <v>60</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>5</v>
@@ -2633,11 +2638,11 @@
       <c r="D76" s="2">
         <v>0</v>
       </c>
-      <c r="E76" s="2"/>
+      <c r="E76" s="6"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>5</v>
@@ -2651,7 +2656,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>5</v>
@@ -2662,11 +2667,11 @@
       <c r="D78" s="2">
         <v>0</v>
       </c>
-      <c r="E78" s="2"/>
+      <c r="E78" s="6"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>5</v>
@@ -2680,7 +2685,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>5</v>
@@ -2691,11 +2696,11 @@
       <c r="D80" s="2">
         <v>0</v>
       </c>
-      <c r="E80" s="2"/>
+      <c r="E80" s="6"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>5</v>
@@ -2709,7 +2714,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>5</v>
@@ -2720,11 +2725,11 @@
       <c r="D82" s="2">
         <v>0</v>
       </c>
-      <c r="E82" s="2"/>
+      <c r="E82" s="6"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>5</v>
@@ -2738,7 +2743,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>5</v>
@@ -2749,11 +2754,11 @@
       <c r="D84" s="2">
         <v>0</v>
       </c>
-      <c r="E84" s="2"/>
+      <c r="E84" s="6"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>5</v>
@@ -2767,10 +2772,10 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>9</v>
@@ -2778,14 +2783,14 @@
       <c r="D86" s="2">
         <v>0</v>
       </c>
-      <c r="E86" s="2"/>
+      <c r="E86" s="6"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>9</v>
@@ -2796,10 +2801,10 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>9</v>
@@ -2807,14 +2812,14 @@
       <c r="D88" s="2">
         <v>0</v>
       </c>
-      <c r="E88" s="2"/>
+      <c r="E88" s="6"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>9</v>
@@ -2823,12 +2828,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>9</v>
@@ -2836,14 +2841,16 @@
       <c r="D90" s="2">
         <v>0</v>
       </c>
-      <c r="E90" s="2"/>
+      <c r="E90" s="7" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>9</v>
@@ -2854,22 +2861,22 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>91</v>
+        <v>174</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D92" s="2">
         <v>0</v>
       </c>
-      <c r="E92" s="2"/>
+      <c r="E92" s="6"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>11</v>
@@ -2883,7 +2890,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>11</v>
@@ -2894,11 +2901,11 @@
       <c r="D94" s="2">
         <v>0</v>
       </c>
-      <c r="E94" s="2"/>
+      <c r="E94" s="6"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>11</v>
@@ -2912,10 +2919,10 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>9</v>
@@ -2923,17 +2930,17 @@
       <c r="D96" s="2">
         <v>0</v>
       </c>
-      <c r="E96" s="2"/>
+      <c r="E96" s="6"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="D97" s="1">
         <v>0</v>
@@ -2941,57 +2948,60 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="D98" s="2">
         <v>0</v>
       </c>
-      <c r="E98" s="2"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E98" s="6"/>
+    </row>
+    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="D99" s="1">
         <v>0</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="D100" s="2">
         <v>0</v>
       </c>
-      <c r="E100" s="2"/>
+      <c r="E100" s="6"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D101" s="1">
         <v>0</v>
@@ -2999,60 +3009,57 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D102" s="2">
         <v>0</v>
       </c>
-      <c r="E102" s="2"/>
+      <c r="E102" s="6"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D103" s="1">
         <v>0</v>
-      </c>
-      <c r="E103" s="5" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D104" s="2">
         <v>0</v>
       </c>
-      <c r="E104" s="2"/>
+      <c r="E104" s="6"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D105" s="1">
         <v>0</v>
@@ -3060,28 +3067,28 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D106" s="2">
         <v>0</v>
       </c>
-      <c r="E106" s="2"/>
+      <c r="E106" s="6"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D107" s="1">
         <v>0</v>
@@ -3089,28 +3096,28 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D108" s="2">
         <v>0</v>
       </c>
-      <c r="E108" s="2"/>
+      <c r="E108" s="6"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D109" s="1">
         <v>0</v>
@@ -3118,28 +3125,28 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D110" s="2">
         <v>0</v>
       </c>
-      <c r="E110" s="2"/>
+      <c r="E110" s="6"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D111" s="1">
         <v>0</v>
@@ -3147,28 +3154,28 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D112" s="2">
         <v>0</v>
       </c>
-      <c r="E112" s="2"/>
+      <c r="E112" s="6"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D113" s="1">
         <v>0</v>
@@ -3176,28 +3183,28 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D114" s="2">
         <v>0</v>
       </c>
-      <c r="E114" s="2"/>
+      <c r="E114" s="6"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D115" s="1">
         <v>0</v>
@@ -3205,28 +3212,28 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D116" s="2">
         <v>0</v>
       </c>
-      <c r="E116" s="2"/>
+      <c r="E116" s="6"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D117" s="1">
         <v>0</v>
@@ -3234,28 +3241,28 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D118" s="2">
         <v>0</v>
       </c>
-      <c r="E118" s="2"/>
+      <c r="E118" s="6"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D119" s="1">
         <v>0</v>
@@ -3263,28 +3270,28 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="D120" s="2">
         <v>0</v>
       </c>
-      <c r="E120" s="2"/>
+      <c r="E120" s="6"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="D121" s="1">
         <v>0</v>
@@ -3292,28 +3299,28 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="D122" s="2">
         <v>0</v>
       </c>
-      <c r="E122" s="2"/>
+      <c r="E122" s="6"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="D123" s="1">
         <v>0</v>
@@ -3321,7 +3328,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>5</v>
@@ -3332,11 +3339,11 @@
       <c r="D124" s="2">
         <v>0</v>
       </c>
-      <c r="E124" s="2"/>
+      <c r="E124" s="6"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>5</v>
@@ -3350,28 +3357,28 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D126" s="2">
         <v>0</v>
       </c>
-      <c r="E126" s="2"/>
+      <c r="E126" s="6"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>127</v>
+        <v>183</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D127" s="1">
         <v>0</v>
@@ -3379,36 +3386,36 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D128" s="2">
-        <v>0</v>
-      </c>
-      <c r="E128" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="D128" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D129" s="1">
-        <v>0</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D129" s="2">
+        <v>0</v>
+      </c>
+      <c r="E129" s="6"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>5</v>
@@ -3419,11 +3426,11 @@
       <c r="D130" s="2">
         <v>0</v>
       </c>
-      <c r="E130" s="2"/>
+      <c r="E130" s="6"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>5</v>
@@ -3437,28 +3444,28 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D132" s="2">
         <v>0</v>
       </c>
-      <c r="E132" s="2"/>
+      <c r="E132" s="6"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D133" s="1">
         <v>0</v>
@@ -3466,7 +3473,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>5</v>
@@ -3477,17 +3484,17 @@
       <c r="D134" s="2">
         <v>0</v>
       </c>
-      <c r="E134" s="2"/>
+      <c r="E134" s="6"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D135" s="1">
         <v>0</v>
@@ -3495,7 +3502,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>5</v>
@@ -3506,17 +3513,17 @@
       <c r="D136" s="2">
         <v>0</v>
       </c>
-      <c r="E136" s="2"/>
+      <c r="E136" s="6"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D137" s="1">
         <v>0</v>
@@ -3524,28 +3531,28 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D138" s="2">
         <v>0</v>
       </c>
-      <c r="E138" s="2"/>
+      <c r="E138" s="6"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D139" s="1">
         <v>0</v>
@@ -3553,10 +3560,10 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>9</v>
@@ -3564,14 +3571,14 @@
       <c r="D140" s="2">
         <v>0</v>
       </c>
-      <c r="E140" s="2"/>
+      <c r="E140" s="6"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>9</v>
@@ -3582,28 +3589,28 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D142" s="2">
         <v>0</v>
       </c>
-      <c r="E142" s="2"/>
+      <c r="E142" s="6"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D143" s="1">
         <v>0</v>
@@ -3611,28 +3618,28 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D144" s="2">
         <v>0</v>
       </c>
-      <c r="E144" s="2"/>
+      <c r="E144" s="6"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D145" s="1">
         <v>0</v>
@@ -3640,10 +3647,10 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>146</v>
+        <v>189</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>12</v>
@@ -3651,17 +3658,17 @@
       <c r="D146" s="2">
         <v>0</v>
       </c>
-      <c r="E146" s="2"/>
+      <c r="E146" s="6"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D147" s="1">
         <v>0</v>
@@ -3669,28 +3676,28 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D148" s="2">
         <v>0</v>
       </c>
-      <c r="E148" s="2"/>
+      <c r="E148" s="6"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D149" s="1">
         <v>0</v>
@@ -3698,10 +3705,10 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>9</v>
@@ -3709,17 +3716,17 @@
       <c r="D150" s="2">
         <v>0</v>
       </c>
-      <c r="E150" s="2"/>
+      <c r="E150" s="6"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D151" s="1">
         <v>0</v>
@@ -3727,22 +3734,22 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D152" s="2">
         <v>0</v>
       </c>
-      <c r="E152" s="2"/>
+      <c r="E152" s="6"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>5</v>
@@ -3750,245 +3757,151 @@
       <c r="C153" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D153" s="1">
-        <v>0</v>
-      </c>
+      <c r="D153" s="2">
+        <v>0</v>
+      </c>
+      <c r="E153" s="6"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D154" s="2">
-        <v>0</v>
-      </c>
-      <c r="E154" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="D154" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D155" s="1">
-        <v>0</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D155" s="2">
+        <v>0</v>
+      </c>
+      <c r="E155" s="6"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D156" s="2">
-        <v>0</v>
-      </c>
-      <c r="E156" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="D156" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D157" s="1">
-        <v>0</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D157" s="2">
+        <v>0</v>
+      </c>
+      <c r="E157" s="6"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D158" s="2">
-        <v>0</v>
-      </c>
-      <c r="E158" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="D158" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D159" s="1">
-        <v>0</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D159" s="2">
+        <v>0</v>
+      </c>
+      <c r="E159" s="6"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D160" s="2">
-        <v>0</v>
-      </c>
-      <c r="E160" s="2"/>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D160" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D161" s="1">
-        <v>0</v>
+        <v>81</v>
+      </c>
+      <c r="D161" s="2">
+        <v>0</v>
+      </c>
+      <c r="E161" s="7" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D162" s="2">
-        <v>0</v>
-      </c>
-      <c r="E162" s="2"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A163" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D163" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D164" s="2">
-        <v>0</v>
-      </c>
-      <c r="E164" s="2"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A165" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D165" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A166" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D166" s="2">
-        <v>0</v>
-      </c>
-      <c r="E166" s="2"/>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A167" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D167" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A168" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D168" s="2">
-        <v>0</v>
-      </c>
-      <c r="E168" s="2"/>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A169" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D169" s="1">
+        <v>81</v>
+      </c>
+      <c r="D162" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E103" r:id="rId1"/>
+    <hyperlink ref="E99" r:id="rId1"/>
+    <hyperlink ref="E41" r:id="rId2"/>
+    <hyperlink ref="E161" r:id="rId3"/>
+    <hyperlink ref="E90" r:id="rId4"/>
+    <hyperlink ref="E58" r:id="rId5"/>
+    <hyperlink ref="E57" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>